<commit_message>
Adding all updated files
</commit_message>
<xml_diff>
--- a/Excel_Files/No of Job Seekers.xlsx
+++ b/Excel_Files/No of Job Seekers.xlsx
@@ -15,6 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet0" r:id="rId5" sheetId="2"/>
     <sheet name="Sheet2" r:id="rId6" sheetId="3"/>
+    <sheet name="Sheet3" r:id="rId7" sheetId="4"/>
+    <sheet name="Sheet4" r:id="rId8" sheetId="5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t>No of Job Seekers</t>
   </si>
@@ -391,4 +393,38 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>